<commit_message>
Added services to upload images as a zip file
</commit_message>
<xml_diff>
--- a/business/catalogue-service-micro/src/main/resources/template/cradle_filled.xlsx
+++ b/business/catalogue-service-micro/src/main/resources/template/cradle_filled.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suat\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\srdc\projects\NIMBLE\project_starts\WP3\T3.2\publishin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10050" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="132">
   <si>
     <t>How to fill in this template?</t>
   </si>
@@ -161,18 +161,15 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Images</t>
+    <t>Certifications</t>
+  </si>
+  <si>
+    <t>Product Data Sheet</t>
   </si>
   <si>
     <t>FILE</t>
   </si>
   <si>
-    <t>Certifications</t>
-  </si>
-  <si>
-    <t>Product Data Sheet</t>
-  </si>
-  <si>
     <t>Product Safety Sheet</t>
   </si>
   <si>
@@ -308,6 +305,9 @@
     <t>Estimated Delivery Period</t>
   </si>
   <si>
+    <t>Applicable Address Country</t>
+  </si>
+  <si>
     <t>Transport Mode</t>
   </si>
   <si>
@@ -344,10 +344,7 @@
     <t>Data Type</t>
   </si>
   <si>
-    <t>INT</t>
-  </si>
-  <si>
-    <t>FLOAT</t>
+    <t>REAL_MEASURE</t>
   </si>
   <si>
     <t>http://www.aidimme.es/FurnitureSectorOntology.owl#Cradle</t>
@@ -356,28 +353,61 @@
     <t>FurnitureOntology</t>
   </si>
   <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>week</t>
+  </si>
+  <si>
     <t>globitowhite</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Carton brick</t>
+  </si>
+  <si>
+    <t>nicolewhite</t>
+  </si>
+  <si>
+    <t>Spain|France|Portugal</t>
+  </si>
+  <si>
+    <t>Road</t>
+  </si>
+  <si>
+    <t>Delivery special terms</t>
+  </si>
+  <si>
+    <t>CIP</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
     <t>Globito White</t>
   </si>
   <si>
     <t>An original design that combines straight lines of the side rails with a rounded head board on this cradle of 120 x 60. Robust but with a light aspect at the same time, it is ideal for the sleep of the youngest.</t>
   </si>
   <si>
-    <t>day</t>
-  </si>
-  <si>
-    <t>cm</t>
-  </si>
-  <si>
-    <t>kg</t>
-  </si>
-  <si>
     <t>Spain</t>
   </si>
   <si>
-    <t>nicolewhite</t>
+    <t>8431830130773</t>
+  </si>
+  <si>
+    <t>White</t>
   </si>
   <si>
     <t>Nicole White</t>
@@ -386,38 +416,17 @@
     <t>Nicole is a classic and elegant cradle, which remains current with the passage of time. Available in four colours of wood: white, honey, natural and chocolate. Optional drawer.</t>
   </si>
   <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>Carton brick</t>
-  </si>
-  <si>
-    <t>week</t>
-  </si>
-  <si>
-    <t>C:\Users\suat\Desktop\nicole_white1.jpg|C:\Users\suat\Desktop\nicole_white2.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\suat\Desktop\globito_white.jpg</t>
+    <t>color</t>
+  </si>
+  <si>
+    <t>Eco label|ISO 9001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -439,12 +448,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -472,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -482,9 +485,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -995,10 +997,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AH6"/>
+  <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1007,67 +1009,66 @@
     <col min="2" max="2" width="31.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="33.90625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.54296875" customWidth="1"/>
-    <col min="29" max="29" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="I1" s="8" t="s">
+    <row r="1" spans="1:33" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="8" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="9"/>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="9"/>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="9"/>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
@@ -1084,7 +1085,7 @@
         <v>45</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>48</v>
@@ -1093,7 +1094,7 @@
         <v>49</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>52</v>
@@ -1102,10 +1103,10 @@
         <v>53</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>58</v>
@@ -1164,14 +1165,11 @@
       <c r="AF2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="AG2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH2" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AG2" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -1185,98 +1183,95 @@
         <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M3" t="s">
         <v>41</v>
-      </c>
-      <c r="G3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L3" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" t="s">
-        <v>57</v>
       </c>
       <c r="N3" t="s">
         <v>41</v>
       </c>
       <c r="O3" t="s">
+        <v>54</v>
+      </c>
+      <c r="P3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" t="s">
         <v>41</v>
       </c>
-      <c r="P3" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>55</v>
-      </c>
-      <c r="R3" t="s">
-        <v>55</v>
-      </c>
       <c r="S3" t="s">
+        <v>54</v>
+      </c>
+      <c r="T3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V3" t="s">
         <v>41</v>
       </c>
-      <c r="T3" t="s">
-        <v>55</v>
-      </c>
-      <c r="U3" t="s">
-        <v>55</v>
-      </c>
-      <c r="V3" t="s">
-        <v>55</v>
-      </c>
       <c r="W3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y3" t="s">
         <v>41</v>
       </c>
-      <c r="X3" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>57</v>
-      </c>
       <c r="Z3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA3" t="s">
         <v>41</v>
       </c>
-      <c r="AA3" t="s">
-        <v>57</v>
-      </c>
       <c r="AB3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG3" t="s">
         <v>41</v>
       </c>
-      <c r="AC3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B4" t="s">
@@ -1288,9 +1283,6 @@
       <c r="D4" t="s">
         <v>42</v>
       </c>
-      <c r="E4" t="s">
-        <v>42</v>
-      </c>
       <c r="F4" t="s">
         <v>42</v>
       </c>
@@ -1307,10 +1299,7 @@
         <v>42</v>
       </c>
       <c r="K4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L4" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="M4" t="s">
         <v>42</v>
@@ -1319,25 +1308,25 @@
         <v>42</v>
       </c>
       <c r="O4" t="s">
-        <v>42</v>
+        <v>121</v>
       </c>
       <c r="P4" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>114</v>
+        <v>121</v>
+      </c>
+      <c r="R4" t="s">
+        <v>42</v>
       </c>
       <c r="S4" t="s">
         <v>42</v>
       </c>
       <c r="T4" t="s">
-        <v>42</v>
+        <v>122</v>
       </c>
       <c r="U4" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="V4" t="s">
-        <v>114</v>
+        <v>42</v>
       </c>
       <c r="W4" t="s">
         <v>42</v>
@@ -1369,144 +1358,140 @@
       <c r="AF4" t="s">
         <v>42</v>
       </c>
-      <c r="AG4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="E5" t="s">
-        <v>128</v>
-      </c>
-      <c r="L5">
+        <v>131</v>
+      </c>
+      <c r="K5">
         <v>14</v>
       </c>
-      <c r="M5" t="b">
+      <c r="L5" t="b">
         <v>1</v>
       </c>
+      <c r="O5">
+        <v>66</v>
+      </c>
       <c r="P5">
-        <v>66</v>
-      </c>
-      <c r="Q5">
         <v>98</v>
       </c>
+      <c r="T5">
+        <v>26</v>
+      </c>
       <c r="U5">
-        <v>26</v>
-      </c>
-      <c r="V5">
         <v>120</v>
       </c>
-      <c r="X5" t="b">
+      <c r="W5" t="b">
         <v>0</v>
       </c>
-      <c r="Z5" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA5" t="b">
+      <c r="Y5" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z5" t="b">
         <v>0</v>
       </c>
-      <c r="AB5" s="6">
-        <v>8431830130773</v>
-      </c>
-      <c r="AC5" t="b">
+      <c r="AA5" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB5" t="b">
         <v>0</v>
       </c>
-      <c r="AD5">
+      <c r="AC5">
         <v>4</v>
+      </c>
+      <c r="AE5" t="b">
+        <v>1</v>
       </c>
       <c r="AF5" t="b">
         <v>1</v>
       </c>
-      <c r="AG5" t="b">
+      <c r="AG5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" t="s">
+        <v>131</v>
+      </c>
+      <c r="K6">
+        <v>14</v>
+      </c>
+      <c r="L6" t="b">
         <v>1</v>
       </c>
-      <c r="AH5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="O6">
+        <v>66</v>
+      </c>
+      <c r="P6">
+        <v>98</v>
+      </c>
+      <c r="T6">
+        <v>20.5</v>
+      </c>
+      <c r="U6">
+        <v>122</v>
+      </c>
+      <c r="W6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>4</v>
+      </c>
+      <c r="AE6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG6" t="s">
         <v>127</v>
-      </c>
-      <c r="L6">
-        <v>14</v>
-      </c>
-      <c r="M6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P6">
-        <v>66</v>
-      </c>
-      <c r="Q6">
-        <v>98</v>
-      </c>
-      <c r="U6">
-        <v>20.5</v>
-      </c>
-      <c r="V6">
-        <v>122</v>
-      </c>
-      <c r="X6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="6">
-        <v>8431830130773</v>
-      </c>
-      <c r="AC6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD6">
-        <v>4</v>
-      </c>
-      <c r="AF6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:AG1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:AF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1522,34 +1507,36 @@
     <col min="9" max="9" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C1" s="10" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C1" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="9"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O1" s="8"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
@@ -1557,63 +1544,66 @@
         <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
         <v>41</v>
@@ -1625,7 +1615,7 @@
         <v>41</v>
       </c>
       <c r="K3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L3" t="s">
         <v>41</v>
@@ -1634,30 +1624,33 @@
         <v>41</v>
       </c>
       <c r="N3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="F4" t="s">
         <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -1669,18 +1662,21 @@
         <v>42</v>
       </c>
       <c r="K4" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="L4" t="s">
         <v>42</v>
       </c>
       <c r="N4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B5" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
+      </c>
+      <c r="O4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>112</v>
       </c>
       <c r="C5">
         <v>400</v>
@@ -1692,24 +1688,39 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
+      <c r="H5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" t="s">
+        <v>119</v>
+      </c>
+      <c r="J5" t="s">
+        <v>118</v>
+      </c>
       <c r="K5">
         <v>2</v>
       </c>
-      <c r="M5" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="N5">
+      <c r="L5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M5" t="s">
+        <v>117</v>
+      </c>
+      <c r="N5" t="s">
+        <v>114</v>
+      </c>
+      <c r="O5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B6" s="5" t="s">
-        <v>117</v>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>115</v>
       </c>
       <c r="C6">
         <v>250</v>
@@ -1721,18 +1732,33 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
+      <c r="H6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" t="s">
+        <v>119</v>
+      </c>
+      <c r="J6" t="s">
+        <v>118</v>
+      </c>
       <c r="K6">
         <v>2</v>
       </c>
-      <c r="M6" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="N6">
+      <c r="L6" t="s">
+        <v>116</v>
+      </c>
+      <c r="M6" t="s">
+        <v>117</v>
+      </c>
+      <c r="N6" t="s">
+        <v>114</v>
+      </c>
+      <c r="O6">
         <v>1</v>
       </c>
     </row>
@@ -1740,8 +1766,8 @@
   <mergeCells count="4">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="N1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1765,7 +1791,7 @@
     <col min="8" max="8" width="5.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
@@ -1801,11 +1827,11 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="4"/>
       <c r="F2" s="4"/>
@@ -1817,9 +1843,9 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="9"/>
+      <c r="A3" s="8"/>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="4"/>
       <c r="F3" s="4"/>
@@ -1827,13 +1853,13 @@
         <v>42</v>
       </c>
       <c r="K3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="8"/>
+      <c r="B4" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
-      <c r="B4" t="s">
-        <v>58</v>
       </c>
       <c r="D4" s="4"/>
       <c r="F4" s="4"/>
@@ -1841,13 +1867,13 @@
         <v>42</v>
       </c>
       <c r="K4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="9"/>
+      <c r="A5" s="8"/>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="4"/>
       <c r="F5" s="4"/>
@@ -1855,13 +1881,13 @@
         <v>42</v>
       </c>
       <c r="K5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
+      <c r="A6" s="8"/>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="4"/>
       <c r="F6" s="4"/>
@@ -1869,13 +1895,13 @@
         <v>42</v>
       </c>
       <c r="K6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
+      <c r="A7" s="8"/>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="4"/>
       <c r="F7" s="4"/>
@@ -1883,13 +1909,13 @@
         <v>42</v>
       </c>
       <c r="K7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
+      <c r="A8" s="8"/>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="4"/>
       <c r="F8" s="4"/>
@@ -1897,13 +1923,13 @@
         <v>42</v>
       </c>
       <c r="K8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="9"/>
+      <c r="A9" s="8"/>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D9" s="4"/>
       <c r="F9" s="4"/>
@@ -1911,13 +1937,13 @@
         <v>42</v>
       </c>
       <c r="K9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
+      <c r="A10" s="8"/>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10" s="4"/>
       <c r="F10" s="4"/>
@@ -1929,9 +1955,9 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
+      <c r="A11" s="8"/>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="4"/>
       <c r="F11" s="4"/>
@@ -1939,13 +1965,13 @@
         <v>42</v>
       </c>
       <c r="K11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
+      <c r="A12" s="8"/>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="4"/>
       <c r="F12" s="4"/>
@@ -1953,13 +1979,13 @@
         <v>42</v>
       </c>
       <c r="K12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="9"/>
+      <c r="A13" s="8"/>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" s="4"/>
       <c r="F13" s="4"/>
@@ -1967,13 +1993,13 @@
         <v>42</v>
       </c>
       <c r="K13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="9"/>
+      <c r="A14" s="8"/>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14" s="4"/>
       <c r="F14" s="4"/>
@@ -1981,13 +2007,13 @@
         <v>42</v>
       </c>
       <c r="K14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="9"/>
+      <c r="A15" s="8"/>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="4"/>
       <c r="F15" s="4"/>
@@ -1995,13 +2021,13 @@
         <v>42</v>
       </c>
       <c r="K15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
+      <c r="A16" s="8"/>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="4"/>
       <c r="F16" s="4"/>
@@ -2009,13 +2035,13 @@
         <v>42</v>
       </c>
       <c r="K16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="9"/>
+      <c r="A17" s="8"/>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" s="4"/>
       <c r="F17" s="4"/>
@@ -2023,13 +2049,13 @@
         <v>42</v>
       </c>
       <c r="K17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
+      <c r="A18" s="8"/>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D18" s="4"/>
       <c r="F18" s="4"/>
@@ -2037,13 +2063,13 @@
         <v>42</v>
       </c>
       <c r="K18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="9"/>
+      <c r="A19" s="8"/>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D19" s="4"/>
       <c r="F19" s="4"/>
@@ -2051,13 +2077,13 @@
         <v>42</v>
       </c>
       <c r="K19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="9"/>
+      <c r="A20" s="8"/>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="4"/>
       <c r="F20" s="4"/>
@@ -2069,9 +2095,9 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="9"/>
+      <c r="A21" s="8"/>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D21" s="4"/>
       <c r="F21" s="4"/>
@@ -2083,9 +2109,9 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="9"/>
+      <c r="A22" s="8"/>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D22" s="4"/>
       <c r="F22" s="4"/>
@@ -2093,13 +2119,13 @@
         <v>42</v>
       </c>
       <c r="K22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="9"/>
+      <c r="A23" s="8"/>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D23" s="4"/>
       <c r="F23" s="4"/>
@@ -2107,7 +2133,7 @@
         <v>42</v>
       </c>
       <c r="K23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2140,12 +2166,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>